<commit_message>
Modification GUI pour prendre en compte le dossier utilisateur.
</commit_message>
<xml_diff>
--- a/SAP/ParaSAP.xlsx
+++ b/SAP/ParaSAP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nobackup\Dev Informatique\GitHub Clone\Datamet\SAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D42EBE0-2C0B-40ED-B17B-E036BD65FC83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE870C2E-C502-451F-9A8A-5AFC929CB6A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZCMT" sheetId="7" r:id="rId1"/>
@@ -2142,58 +2142,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2360,6 +2308,58 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2374,11 +2374,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B4A09F38-11C0-45C6-97EF-3B2DDC9AA5A7}" name="Tab_ZCMT" displayName="Tab_ZCMT" ref="A1:R290" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B4A09F38-11C0-45C6-97EF-3B2DDC9AA5A7}" name="Tab_ZCMT" displayName="Tab_ZCMT" ref="A1:R290" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A1:R290" xr:uid="{94534B11-27DB-4D04-B2C3-B7102A452673}">
     <filterColumn colId="1">
       <filters>
-        <filter val="GRN"/>
+        <filter val="INC"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2386,16 +2386,16 @@
     <tableColumn id="1" xr3:uid="{DA153C34-2CAF-4258-8D6A-A5DD054E6296}" name="Division"/>
     <tableColumn id="2" xr3:uid="{6F4F5BF2-DDBE-443D-AF5B-E12630E9AED5}" name="Famille Essai"/>
     <tableColumn id="3" xr3:uid="{9055EBA6-0B36-405B-9CBF-B29C24246314}" name="Paramètre"/>
-    <tableColumn id="4" xr3:uid="{786499D9-12C1-4BB7-A085-010BA0826CDC}" name="Datamet" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{786499D9-12C1-4BB7-A085-010BA0826CDC}" name="Datamet" dataDxfId="14">
       <calculatedColumnFormula>IF(VLOOKUP(Tab_ZCMT[[#This Row],[Paramètre]],Tab_Para_Datamet[],2,FALSE)=0,"N/A",VLOOKUP(Tab_ZCMT[[#This Row],[Paramètre]],Tab_Para_Datamet[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{4E21B635-86D7-4F1F-953A-AFF5DA472B73}" name="clefFamille_Para" dataDxfId="3">
+    <tableColumn id="17" xr3:uid="{4E21B635-86D7-4F1F-953A-AFF5DA472B73}" name="clefFamille_Para" dataDxfId="13">
       <calculatedColumnFormula>Tab_ZCMT[[#This Row],[Famille Essai]]&amp;Tab_ZCMT[[#This Row],[Paramètre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{7C5B8C85-4927-4E10-8F99-1699CF3ECF9C}" name="Check si existe dans ZES_PARA_CND_V" dataDxfId="1">
+    <tableColumn id="18" xr3:uid="{7C5B8C85-4927-4E10-8F99-1699CF3ECF9C}" name="Check si existe dans ZES_PARA_CND_V" dataDxfId="12">
       <calculatedColumnFormula>NOT(ISERROR(MATCH(Tab_ZCMT[[#This Row],[clefFamille_Para]],Tab_ZES_PARA_CND_V[ClefFamPara],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{692C1397-9DC4-447D-B5B8-4B37983BF618}" name="Check si existe dans ParaT" dataDxfId="2">
+    <tableColumn id="14" xr3:uid="{692C1397-9DC4-447D-B5B8-4B37983BF618}" name="Check si existe dans ParaT" dataDxfId="11">
       <calculatedColumnFormula>NOT(ISERROR(MATCH(Tab_ZCMT[[#This Row],[Paramètre]],Tab_ParaT[Paramètre],0)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{89C13229-2CE2-4638-AD77-75365AD0D2AD}" name="Envoie SAP"/>
@@ -2425,11 +2425,11 @@
   </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{12E8D901-D673-4F71-A392-C9C0DD2F211E}" name="Famille Essai"/>
-    <tableColumn id="2" xr3:uid="{75D6FEA3-6E1C-4866-A96A-520D0576FF29}" name="Paramètre" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{34AC0294-7DA6-4722-A6BD-3171EEB6DA0F}" name="Code valeur paramètre autorisée" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{75D6FEA3-6E1C-4866-A96A-520D0576FF29}" name="Paramètre" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{34AC0294-7DA6-4722-A6BD-3171EEB6DA0F}" name="Code valeur paramètre autorisée" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{ED29998E-9280-4C13-A8C2-B867EC9594DB}" name="Valeur de caractér."/>
     <tableColumn id="5" xr3:uid="{C290962C-807D-414F-830E-61C9F1B010E4}" name="Code valeur paramètre autorisée obsolète"/>
-    <tableColumn id="6" xr3:uid="{732E81FF-2A31-4A87-AD98-DE5224F78456}" name="ClefFamPara" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{732E81FF-2A31-4A87-AD98-DE5224F78456}" name="ClefFamPara" dataDxfId="8">
       <calculatedColumnFormula>Tab_ZES_PARA_CND_V[[#This Row],[Famille Essai]]&amp;Tab_ZES_PARA_CND_V[[#This Row],[Paramètre]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2438,14 +2438,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{83652C6C-97F4-4B68-8736-064F947595BC}" name="Tab_ParaT" displayName="Tab_ParaT" ref="A1:E4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{83652C6C-97F4-4B68-8736-064F947595BC}" name="Tab_ParaT" displayName="Tab_ParaT" ref="A1:E4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:E4" xr:uid="{0338B4E1-6C91-4444-AB4B-3B8DC73413F7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1B5D5ECB-16F4-4546-916B-E278F7B684B8}" name="Famille" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{1B5D5ECB-16F4-4546-916B-E278F7B684B8}" name="Famille" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{A889EEF1-235B-41FC-B939-B038EB7336DD}" name="Paramètre"/>
-    <tableColumn id="3" xr3:uid="{91CC6839-2F6C-4762-8F87-0A056D95AD9C}" name="Valeur SAP" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{3BCCE4FD-619A-4AF3-AE09-87E28A1DE320}" name="Valeur Datamet" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{8B81BB8E-2DEF-4D24-B258-68850DA62087}" name="Clef_FamillePara" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{91CC6839-2F6C-4762-8F87-0A056D95AD9C}" name="Valeur SAP" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{3BCCE4FD-619A-4AF3-AE09-87E28A1DE320}" name="Valeur Datamet" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8B81BB8E-2DEF-4D24-B258-68850DA62087}" name="Clef_FamillePara" dataDxfId="2">
       <calculatedColumnFormula>Tab_ParaT[[#This Row],[Famille]]&amp;Tab_ParaT[[#This Row],[Paramètre]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2473,7 +2473,7 @@
     <sortCondition ref="A1:A140"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BD39DA7E-8BA0-4425-A650-D78D04606CC9}" name="Paramètre" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{BD39DA7E-8BA0-4425-A650-D78D04606CC9}" name="Paramètre" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{FFAC1574-F462-41FE-88C5-5F7951DCCC39}" name="Datamet"/>
     <tableColumn id="3" xr3:uid="{36438C71-E192-4553-B2B8-2E72570937DE}" name="libellé" dataDxfId="0">
       <calculatedColumnFormula>VLOOKUP(Tab_Para_Datamet[[#This Row],[Paramètre]],Tab_ZCMT[[Paramètre]:[FR - Libellé paramètre]],9,FALSE)</calculatedColumnFormula>
@@ -2782,14 +2782,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E34CB9-A3EC-4A5A-BF45-7B7E6E2FA1BD}">
   <dimension ref="A1:R290"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="38.85546875" bestFit="1" customWidth="1"/>
@@ -6147,7 +6148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -6204,7 +6205,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -6261,7 +6262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -6315,7 +6316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -6372,7 +6373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -6426,7 +6427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -6480,7 +6481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -6534,7 +6535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -6588,7 +6589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -6642,7 +6643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -6696,7 +6697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -6750,7 +6751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -6804,7 +6805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -6858,7 +6859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -6912,7 +6913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -6966,7 +6967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -7020,7 +7021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -7074,7 +7075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -7128,7 +7129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -7182,7 +7183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -7236,7 +7237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -7290,7 +7291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -7344,7 +7345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -7398,7 +7399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -7452,7 +7453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -7506,7 +7507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -7560,7 +7561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -7614,7 +7615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -7668,7 +7669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -7726,7 +7727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -7784,7 +7785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -7838,7 +7839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -7892,7 +7893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -7946,7 +7947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>0</v>
       </c>
@@ -8000,7 +8001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -8054,7 +8055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -8108,7 +8109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -8162,7 +8163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -8219,7 +8220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -8273,7 +8274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -8327,7 +8328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -8381,7 +8382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -8435,7 +8436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -8489,7 +8490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>0</v>
       </c>
@@ -8543,7 +8544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -8597,7 +8598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -8651,7 +8652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -8705,7 +8706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>0</v>
       </c>
@@ -8759,7 +8760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -8813,7 +8814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>0</v>
       </c>
@@ -8867,7 +8868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>0</v>
       </c>
@@ -8921,7 +8922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>0</v>
       </c>
@@ -8975,7 +8976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>0</v>
       </c>
@@ -9029,7 +9030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>0</v>
       </c>
@@ -9083,7 +9084,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -9137,7 +9138,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>0</v>
       </c>
@@ -9191,7 +9192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -9245,7 +9246,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="120" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>0</v>
       </c>
@@ -9299,7 +9300,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="121" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -9353,7 +9354,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -9407,7 +9408,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="123" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -9461,7 +9462,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="124" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>0</v>
       </c>
@@ -9515,7 +9516,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -9569,7 +9570,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -9623,7 +9624,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="127" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -9677,7 +9678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -9731,7 +9732,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -9785,7 +9786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>0</v>
       </c>
@@ -9839,7 +9840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -9893,7 +9894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -9947,7 +9948,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="133" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>0</v>
       </c>
@@ -10001,7 +10002,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>0</v>
       </c>
@@ -10055,7 +10056,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="135" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -10109,7 +10110,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -10163,7 +10164,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -10217,7 +10218,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>0</v>
       </c>
@@ -10273,7 +10274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -10327,7 +10328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>0</v>
       </c>
@@ -10381,7 +10382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>0</v>
       </c>
@@ -10435,7 +10436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -10489,7 +10490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>0</v>
       </c>
@@ -10543,7 +10544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -10597,7 +10598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -10651,7 +10652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -10705,7 +10706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -10759,7 +10760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -10813,7 +10814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -10867,7 +10868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -10921,7 +10922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -10975,7 +10976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -11029,7 +11030,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>0</v>
       </c>
@@ -11083,7 +11084,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="154" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>0</v>
       </c>
@@ -11137,7 +11138,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -11191,7 +11192,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>0</v>
       </c>
@@ -11245,7 +11246,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="157" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -11299,7 +11300,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -11353,7 +11354,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -11407,7 +11408,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>0</v>
       </c>
@@ -11461,7 +11462,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>0</v>
       </c>
@@ -11515,7 +11516,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -11569,7 +11570,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="163" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>0</v>
       </c>
@@ -11623,7 +11624,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -11677,7 +11678,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>0</v>
       </c>
@@ -11731,7 +11732,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>0</v>
       </c>
@@ -11785,7 +11786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -11839,7 +11840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -18500,7 +18501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4492C884-1F45-4DBB-B553-2EC324CDD14A}">
   <dimension ref="A1:F954"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D340" sqref="D340"/>
     </sheetView>
   </sheetViews>
@@ -38752,7 +38753,7 @@
   <dimension ref="A1:C140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
avancement sur norme NORSOK
</commit_message>
<xml_diff>
--- a/SAP/ParaSAP.xlsx
+++ b/SAP/ParaSAP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nobackup\Dev Informatique\GitHub Clone\Datamet\SAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E54397D-4B42-4A7A-87D3-58A6DE38B8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA4CE72-E1E8-46DC-8408-8F69825979E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZCMT" sheetId="7" r:id="rId1"/>
@@ -2203,29 +2203,6 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2382,6 +2359,25 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -2407,6 +2403,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2472,16 +2472,16 @@
     <tableColumn id="4" xr3:uid="{786499D9-12C1-4BB7-A085-010BA0826CDC}" name="Datamet résultat" dataDxfId="17">
       <calculatedColumnFormula>IF(VLOOKUP(Tab_ZCMT[[#This Row],[Paramètre]],Tab_Para_Datamet[],2,FALSE)=0,"N/A",VLOOKUP(Tab_ZCMT[[#This Row],[Paramètre]],Tab_Para_Datamet[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{B20A9FC6-D15D-4CC3-B8DF-F946D195530F}" name="Datamet mesure" dataDxfId="0">
+    <tableColumn id="20" xr3:uid="{B20A9FC6-D15D-4CC3-B8DF-F946D195530F}" name="Datamet mesure" dataDxfId="16">
       <calculatedColumnFormula>IF(VLOOKUP(Tab_ZCMT[[#This Row],[Paramètre]],Tab_Para_Datamet[],3,FALSE)=0,"N/A",VLOOKUP(Tab_ZCMT[[#This Row],[Paramètre]],Tab_Para_Datamet[],3,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{4E21B635-86D7-4F1F-953A-AFF5DA472B73}" name="clefFamille_Para" dataDxfId="16">
+    <tableColumn id="17" xr3:uid="{4E21B635-86D7-4F1F-953A-AFF5DA472B73}" name="clefFamille_Para" dataDxfId="15">
       <calculatedColumnFormula>Tab_ZCMT[[#This Row],[Famille Essai]]&amp;Tab_ZCMT[[#This Row],[Paramètre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{7C5B8C85-4927-4E10-8F99-1699CF3ECF9C}" name="Check si existe dans ZES_PARA_CND_V" dataDxfId="15">
+    <tableColumn id="18" xr3:uid="{7C5B8C85-4927-4E10-8F99-1699CF3ECF9C}" name="Check si existe dans ZES_PARA_CND_V" dataDxfId="14">
       <calculatedColumnFormula>NOT(ISERROR(MATCH(Tab_ZCMT[[#This Row],[clefFamille_Para]],Tab_ZES_PARA_CND_V[ClefFamPara],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{692C1397-9DC4-447D-B5B8-4B37983BF618}" name="Check si existe dans ParaT" dataDxfId="14">
+    <tableColumn id="14" xr3:uid="{692C1397-9DC4-447D-B5B8-4B37983BF618}" name="Check si existe dans ParaT" dataDxfId="13">
       <calculatedColumnFormula>NOT(ISERROR(MATCH(Tab_ZCMT[[#This Row],[Paramètre]],Tab_ParaT[Paramètre],0)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{89C13229-2CE2-4638-AD77-75365AD0D2AD}" name="Envoie SAP"/>
@@ -2511,11 +2511,11 @@
   </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{12E8D901-D673-4F71-A392-C9C0DD2F211E}" name="Famille Essai"/>
-    <tableColumn id="2" xr3:uid="{75D6FEA3-6E1C-4866-A96A-520D0576FF29}" name="Paramètre" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{34AC0294-7DA6-4722-A6BD-3171EEB6DA0F}" name="Code valeur paramètre autorisée" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{75D6FEA3-6E1C-4866-A96A-520D0576FF29}" name="Paramètre" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{34AC0294-7DA6-4722-A6BD-3171EEB6DA0F}" name="Code valeur paramètre autorisée" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{ED29998E-9280-4C13-A8C2-B867EC9594DB}" name="Valeur de caractér."/>
     <tableColumn id="5" xr3:uid="{C290962C-807D-414F-830E-61C9F1B010E4}" name="Code valeur paramètre autorisée obsolète"/>
-    <tableColumn id="6" xr3:uid="{732E81FF-2A31-4A87-AD98-DE5224F78456}" name="ClefFamPara" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{732E81FF-2A31-4A87-AD98-DE5224F78456}" name="ClefFamPara" dataDxfId="10">
       <calculatedColumnFormula>Tab_ZES_PARA_CND_V[[#This Row],[Famille Essai]]&amp;Tab_ZES_PARA_CND_V[[#This Row],[Paramètre]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2524,14 +2524,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{83652C6C-97F4-4B68-8736-064F947595BC}" name="Tab_ParaT" displayName="Tab_ParaT" ref="A1:E3" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{83652C6C-97F4-4B68-8736-064F947595BC}" name="Tab_ParaT" displayName="Tab_ParaT" ref="A1:E3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:E3" xr:uid="{0338B4E1-6C91-4444-AB4B-3B8DC73413F7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1B5D5ECB-16F4-4546-916B-E278F7B684B8}" name="Famille" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1B5D5ECB-16F4-4546-916B-E278F7B684B8}" name="Famille" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{A889EEF1-235B-41FC-B939-B038EB7336DD}" name="Paramètre"/>
-    <tableColumn id="3" xr3:uid="{91CC6839-2F6C-4762-8F87-0A056D95AD9C}" name="Valeur SAP" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{3BCCE4FD-619A-4AF3-AE09-87E28A1DE320}" name="Valeur Datamet" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{8B81BB8E-2DEF-4D24-B258-68850DA62087}" name="Clef_FamillePara" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{91CC6839-2F6C-4762-8F87-0A056D95AD9C}" name="Valeur SAP" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{3BCCE4FD-619A-4AF3-AE09-87E28A1DE320}" name="Valeur Datamet" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{8B81BB8E-2DEF-4D24-B258-68850DA62087}" name="Clef_FamillePara" dataDxfId="4">
       <calculatedColumnFormula>Tab_ParaT[[#This Row],[Famille]]&amp;Tab_ParaT[[#This Row],[Paramètre]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2559,10 +2559,10 @@
     <sortCondition ref="A1:A140"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BD39DA7E-8BA0-4425-A650-D78D04606CC9}" name="Paramètre" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{BD39DA7E-8BA0-4425-A650-D78D04606CC9}" name="Paramètre" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{FFAC1574-F462-41FE-88C5-5F7951DCCC39}" name="Datamet résultat"/>
     <tableColumn id="4" xr3:uid="{A59910DE-C57B-4EB0-A417-ADDEBFE07B7E}" name="Datamet mesure"/>
-    <tableColumn id="3" xr3:uid="{36438C71-E192-4553-B2B8-2E72570937DE}" name="libellé" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{36438C71-E192-4553-B2B8-2E72570937DE}" name="libellé" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Tab_Para_Datamet[[#This Row],[Paramètre]],Tab_ZCMT[[Paramètre]:[FR - Libellé paramètre]],9,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2577,8 +2577,8 @@
     <tableColumn id="1" xr3:uid="{A46EDBD2-509A-42FC-A2B2-CACE66F30C0E}" name="Nom"/>
     <tableColumn id="2" xr3:uid="{9DE68AD5-848C-4350-94E7-DDB3A9C9A994}" name="FamilleQR"/>
     <tableColumn id="3" xr3:uid="{400A0C43-6936-4183-A412-C717BF4FB8AF}" name="Para SAP"/>
-    <tableColumn id="4" xr3:uid="{6D809447-70B3-40CF-9CBE-CE59123B984D}" name="Datamet module" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E2F91904-20FF-468B-8323-565E60BE7936}" name="Datamet résultat" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{6D809447-70B3-40CF-9CBE-CE59123B984D}" name="Datamet module" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E2F91904-20FF-468B-8323-565E60BE7936}" name="Datamet résultat" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2883,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E34CB9-A3EC-4A5A-BF45-7B7E6E2FA1BD}">
   <dimension ref="A1:T290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="J269" sqref="J269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2896,6 +2896,7 @@
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -18791,7 +18792,7 @@
         <v>0</v>
       </c>
       <c r="J269" t="s">
-        <v>618</v>
+        <v>650</v>
       </c>
       <c r="L269" t="s">
         <v>2</v>
@@ -40312,7 +40313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04208C3-866B-4657-8A40-CF0598CA90CF}">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
en cours : Création du xml pour les images, a finir : nommage des images
</commit_message>
<xml_diff>
--- a/SAP/ParaSAP.xlsx
+++ b/SAP/ParaSAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nobackup\Dev Informatique\GitHub Clone\Datamet\SAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA4CE72-E1E8-46DC-8408-8F69825979E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F6B918-98D5-4CDE-98A8-E66C90EA3088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6131" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6132" uniqueCount="654">
   <si>
     <t>8041</t>
   </si>
@@ -2463,7 +2463,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B4A09F38-11C0-45C6-97EF-3B2DDC9AA5A7}" name="Tab_ZCMT" displayName="Tab_ZCMT" ref="A1:T290" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19">
-  <autoFilter ref="A1:T290" xr:uid="{94534B11-27DB-4D04-B2C3-B7102A452673}"/>
+  <autoFilter ref="A1:T290" xr:uid="{94534B11-27DB-4D04-B2C3-B7102A452673}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="FRC"/>
+        <filter val="STR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{DA153C34-2CAF-4258-8D6A-A5DD054E6296}" name="Division"/>
     <tableColumn id="2" xr3:uid="{6F4F5BF2-DDBE-443D-AF5B-E12630E9AED5}" name="Famille Essai"/>
@@ -2883,8 +2890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E34CB9-A3EC-4A5A-BF45-7B7E6E2FA1BD}">
   <dimension ref="A1:T290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="J269" sqref="J269"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5367,6 +5374,9 @@
         <f>NOT(ISERROR(MATCH(Tab_ZCMT[[#This Row],[Paramètre]],Tab_ParaT[Paramètre],0)))</f>
         <v>0</v>
       </c>
+      <c r="J42" t="s">
+        <v>650</v>
+      </c>
       <c r="L42" t="s">
         <v>2</v>
       </c>
@@ -6575,7 +6585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -6637,7 +6647,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -6699,7 +6709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -6758,7 +6768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -6820,7 +6830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -6879,7 +6889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -6938,7 +6948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -6997,7 +7007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -7056,7 +7066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -7115,7 +7125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -7174,7 +7184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -7233,7 +7243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -7292,7 +7302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -7351,7 +7361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -7410,7 +7420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -7469,7 +7479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -7528,7 +7538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -7587,7 +7597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -7646,7 +7656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -7705,7 +7715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -7764,7 +7774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -7823,7 +7833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -7882,7 +7892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -7941,7 +7951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -8000,7 +8010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -8059,7 +8069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -8118,7 +8128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -8177,7 +8187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -8236,7 +8246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -8299,7 +8309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -8362,7 +8372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -8421,7 +8431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -8480,7 +8490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -8539,7 +8549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>0</v>
       </c>
@@ -8598,7 +8608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -8657,7 +8667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -8716,7 +8726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -8775,7 +8785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -8837,7 +8847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -8896,7 +8906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -8955,7 +8965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -9014,7 +9024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -9073,7 +9083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -9132,7 +9142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>0</v>
       </c>
@@ -9191,7 +9201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -9250,7 +9260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -9309,7 +9319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -9368,7 +9378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>0</v>
       </c>
@@ -9427,7 +9437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -9486,7 +9496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>0</v>
       </c>
@@ -9545,7 +9555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>0</v>
       </c>
@@ -9604,7 +9614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>0</v>
       </c>
@@ -9663,7 +9673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>0</v>
       </c>
@@ -9722,7 +9732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>0</v>
       </c>
@@ -9781,7 +9791,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -9840,7 +9850,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>0</v>
       </c>
@@ -9899,7 +9909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -9958,7 +9968,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>0</v>
       </c>
@@ -10017,7 +10027,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -10076,7 +10086,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -10135,7 +10145,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -10194,7 +10204,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>0</v>
       </c>
@@ -10253,7 +10263,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -10312,7 +10322,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -10371,7 +10381,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -10430,7 +10440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -10489,7 +10499,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -10548,7 +10558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>0</v>
       </c>
@@ -10607,7 +10617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -10666,7 +10676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -10725,7 +10735,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>0</v>
       </c>
@@ -10784,7 +10794,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>0</v>
       </c>
@@ -10843,7 +10853,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -10902,7 +10912,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -10961,7 +10971,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -11020,7 +11030,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>0</v>
       </c>
@@ -11081,7 +11091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -11140,7 +11150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>0</v>
       </c>
@@ -11199,7 +11209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>0</v>
       </c>
@@ -11258,7 +11268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -11317,7 +11327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>0</v>
       </c>
@@ -11376,7 +11386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -11435,7 +11445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -11494,7 +11504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -11553,7 +11563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -11612,7 +11622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -11671,7 +11681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -11730,7 +11740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -11789,7 +11799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -11848,7 +11858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -11907,7 +11917,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>0</v>
       </c>
@@ -11966,7 +11976,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>0</v>
       </c>
@@ -12025,7 +12035,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -12084,7 +12094,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>0</v>
       </c>
@@ -12143,7 +12153,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -12202,7 +12212,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -12261,7 +12271,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -12320,7 +12330,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>0</v>
       </c>
@@ -12379,7 +12389,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>0</v>
       </c>
@@ -12438,7 +12448,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -12497,7 +12507,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>0</v>
       </c>
@@ -12556,7 +12566,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -12615,7 +12625,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>0</v>
       </c>
@@ -12674,7 +12684,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>0</v>
       </c>
@@ -12733,7 +12743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -12792,7 +12802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -12851,7 +12861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>0</v>
       </c>
@@ -12910,7 +12920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -12969,7 +12979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>0</v>
       </c>
@@ -13028,7 +13038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>0</v>
       </c>
@@ -13087,7 +13097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>0</v>
       </c>
@@ -13146,7 +13156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>0</v>
       </c>
@@ -13205,7 +13215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>0</v>
       </c>
@@ -13264,7 +13274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>0</v>
       </c>
@@ -13323,7 +13333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>0</v>
       </c>
@@ -13382,7 +13392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>0</v>
       </c>
@@ -13441,7 +13451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>0</v>
       </c>
@@ -13500,7 +13510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>0</v>
       </c>
@@ -13559,7 +13569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>0</v>
       </c>
@@ -13618,7 +13628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -13677,7 +13687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>0</v>
       </c>
@@ -13736,7 +13746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>0</v>
       </c>
@@ -13795,7 +13805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -13854,7 +13864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>0</v>
       </c>
@@ -13913,7 +13923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -13972,7 +13982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>0</v>
       </c>
@@ -14031,7 +14041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>0</v>
       </c>
@@ -14090,7 +14100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>0</v>
       </c>
@@ -14149,7 +14159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>0</v>
       </c>
@@ -14208,7 +14218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>0</v>
       </c>
@@ -14267,7 +14277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>0</v>
       </c>
@@ -14326,7 +14336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>0</v>
       </c>
@@ -14385,7 +14395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>0</v>
       </c>
@@ -14446,7 +14456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>0</v>
       </c>
@@ -14505,7 +14515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>0</v>
       </c>
@@ -14564,7 +14574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>0</v>
       </c>
@@ -14623,7 +14633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>0</v>
       </c>
@@ -14682,7 +14692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>0</v>
       </c>
@@ -14741,7 +14751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>0</v>
       </c>
@@ -14800,7 +14810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>0</v>
       </c>
@@ -14859,7 +14869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>0</v>
       </c>
@@ -14918,7 +14928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>0</v>
       </c>
@@ -14977,7 +14987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>0</v>
       </c>
@@ -15036,7 +15046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>0</v>
       </c>
@@ -15095,7 +15105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>0</v>
       </c>
@@ -15154,7 +15164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>0</v>
       </c>
@@ -15213,7 +15223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>0</v>
       </c>
@@ -15272,7 +15282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>0</v>
       </c>
@@ -15331,7 +15341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>0</v>
       </c>
@@ -15390,7 +15400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>0</v>
       </c>
@@ -15449,7 +15459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>0</v>
       </c>
@@ -15508,7 +15518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>0</v>
       </c>
@@ -15567,7 +15577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>0</v>
       </c>
@@ -15626,7 +15636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>0</v>
       </c>
@@ -15685,7 +15695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -15744,7 +15754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>0</v>
       </c>
@@ -15803,7 +15813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>0</v>
       </c>
@@ -15862,7 +15872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>0</v>
       </c>
@@ -15921,7 +15931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>0</v>
       </c>
@@ -15980,7 +15990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>0</v>
       </c>
@@ -16039,7 +16049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>0</v>
       </c>
@@ -16098,7 +16108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>0</v>
       </c>
@@ -16157,7 +16167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>0</v>
       </c>
@@ -16216,7 +16226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>0</v>
       </c>
@@ -16275,7 +16285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -16334,7 +16344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>0</v>
       </c>
@@ -16393,7 +16403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -16452,7 +16462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -16511,7 +16521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -16570,7 +16580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>0</v>
       </c>
@@ -16629,7 +16639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -16688,7 +16698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>0</v>
       </c>
@@ -16747,7 +16757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>0</v>
       </c>
@@ -16806,7 +16816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>0</v>
       </c>
@@ -16865,7 +16875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>0</v>
       </c>
@@ -16924,7 +16934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>0</v>
       </c>
@@ -16983,7 +16993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>0</v>
       </c>
@@ -17042,7 +17052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>0</v>
       </c>
@@ -17101,7 +17111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>0</v>
       </c>
@@ -17160,7 +17170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>0</v>
       </c>
@@ -17219,7 +17229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -17278,7 +17288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>0</v>
       </c>
@@ -17337,7 +17347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>0</v>
       </c>
@@ -17396,7 +17406,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="246" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>0</v>
       </c>
@@ -17455,7 +17465,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="247" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>0</v>
       </c>
@@ -17514,7 +17524,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="248" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>0</v>
       </c>
@@ -17573,7 +17583,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="249" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>0</v>
       </c>
@@ -17632,7 +17642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>0</v>
       </c>
@@ -17691,7 +17701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>0</v>
       </c>
@@ -17750,7 +17760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>0</v>
       </c>
@@ -17809,7 +17819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>0</v>
       </c>
@@ -17868,7 +17878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>0</v>
       </c>
@@ -17927,7 +17937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>0</v>
       </c>
@@ -17986,7 +17996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>0</v>
       </c>
@@ -18045,7 +18055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>0</v>
       </c>
@@ -18104,7 +18114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>0</v>
       </c>
@@ -18163,7 +18173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>0</v>
       </c>
@@ -18222,7 +18232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>0</v>
       </c>
@@ -18281,7 +18291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>0</v>
       </c>

</xml_diff>